<commit_message>
Updated excel file with youtubers
</commit_message>
<xml_diff>
--- a/youtubers.xlsx
+++ b/youtubers.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>Draft ready</t>
+  </si>
+  <si>
+    <t>Sent</t>
   </si>
 </sst>
 </file>
@@ -714,7 +717,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +798,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
         <v>73</v>
@@ -824,7 +827,7 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
         <v>66</v>
@@ -850,7 +853,7 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G5">
         <v>0.2</v>
@@ -870,7 +873,7 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G6">
         <v>1300</v>
@@ -896,7 +899,7 @@
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E7" t="s">
         <v>68</v>
@@ -916,7 +919,7 @@
         <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G8">
         <v>2.2999999999999998</v>
@@ -933,7 +936,7 @@
         <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I9">
         <v>0.2</v>
@@ -950,7 +953,7 @@
         <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
         <v>73</v>
@@ -970,7 +973,7 @@
         <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F11">
         <v>11</v>
@@ -996,7 +999,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F12">
         <v>0.6</v>
@@ -1019,7 +1022,7 @@
         <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F13">
         <v>121</v>
@@ -1045,7 +1048,7 @@
         <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E14" t="s">
         <v>71</v>
@@ -1074,7 +1077,7 @@
         <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F15">
         <v>164</v>
@@ -1097,7 +1100,7 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F16">
         <v>3800</v>
@@ -1117,7 +1120,7 @@
         <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F17">
         <v>7.0000000000000007E-2</v>
@@ -1134,7 +1137,7 @@
         <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E18" t="s">
         <v>72</v>
@@ -1160,7 +1163,7 @@
         <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F19">
         <v>26</v>
@@ -1183,7 +1186,7 @@
         <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F20">
         <v>186</v>
@@ -1200,7 +1203,7 @@
         <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G21">
         <v>2.8</v>
@@ -1220,7 +1223,7 @@
         <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
         <v>74</v>
@@ -1240,7 +1243,7 @@
         <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F23">
         <v>4.8</v>

</xml_diff>

<commit_message>
Prepared release for youtubers
</commit_message>
<xml_diff>
--- a/youtubers.xlsx
+++ b/youtubers.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$35</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="129">
   <si>
     <t>Name</t>
   </si>
@@ -338,10 +341,85 @@
     <t>thesandboxsocial@gmail.com</t>
   </si>
   <si>
-    <t>Draft ready</t>
-  </si>
-  <si>
     <t>Sent</t>
+  </si>
+  <si>
+    <t>Working on key draft</t>
+  </si>
+  <si>
+    <t>Followed up on Twitter</t>
+  </si>
+  <si>
+    <t>Not interested</t>
+  </si>
+  <si>
+    <t>H6AEV-L2M5A-BZLR5</t>
+  </si>
+  <si>
+    <t>LZ599-QL2BT-8GVE2</t>
+  </si>
+  <si>
+    <t>K9ZZ8-8R5TH-BQAYN</t>
+  </si>
+  <si>
+    <t>5KR6C-PB5W5-F06MA</t>
+  </si>
+  <si>
+    <t>WEN9L-WX5XI-RRYA3</t>
+  </si>
+  <si>
+    <t>YJV3C-EMRFJ-C7M7K</t>
+  </si>
+  <si>
+    <t>F3C4X-2WFJK-PF0VJ</t>
+  </si>
+  <si>
+    <t>Q7MV3-94YTH-7AF5X</t>
+  </si>
+  <si>
+    <t>7PLIV-CQWPB-0Z065</t>
+  </si>
+  <si>
+    <t>VIX90-DTXBT-TAEKX</t>
+  </si>
+  <si>
+    <t>PK2JE-V9A0R-9GMG2</t>
+  </si>
+  <si>
+    <t>9FYNF-C3JZ5-RQTD9</t>
+  </si>
+  <si>
+    <t>HN8X9-44FM9-W54AY</t>
+  </si>
+  <si>
+    <t>NYWQ5-DX680-02RR5</t>
+  </si>
+  <si>
+    <t>GHJ05-R2D2Z-3XETD</t>
+  </si>
+  <si>
+    <t>M9EJ6-W4W30-VD8JK</t>
+  </si>
+  <si>
+    <t>W0RIT-FYV2E-3CI6B</t>
+  </si>
+  <si>
+    <t>6ILXL-TR8E8-D2HAW</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Lousterlou</t>
+  </si>
+  <si>
+    <t>KinglyValence</t>
+  </si>
+  <si>
+    <t>Nate Crowley</t>
   </si>
 </sst>
 </file>
@@ -713,11 +791,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +803,7 @@
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
@@ -735,7 +813,7 @@
     <col min="11" max="11" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -769,8 +847,11 @@
       <c r="K1" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -789,8 +870,11 @@
       <c r="H2">
         <v>669</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -815,8 +899,11 @@
       <c r="J3">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -827,7 +914,7 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
         <v>66</v>
@@ -842,7 +929,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -853,7 +940,7 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5">
         <v>0.2</v>
@@ -862,7 +949,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -873,7 +960,7 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G6">
         <v>1300</v>
@@ -888,7 +975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -899,7 +986,7 @@
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
         <v>68</v>
@@ -908,7 +995,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -924,8 +1011,11 @@
       <c r="G8">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -941,8 +1031,11 @@
       <c r="I9">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -964,8 +1057,11 @@
       <c r="I10">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -990,8 +1086,11 @@
       <c r="J11">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1013,8 +1112,11 @@
       <c r="K12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1022,7 +1124,7 @@
         <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F13">
         <v>121</v>
@@ -1037,7 +1139,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1048,7 +1150,7 @@
         <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" t="s">
         <v>71</v>
@@ -1066,7 +1168,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1088,8 +1190,11 @@
       <c r="H15">
         <v>117</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1100,7 +1205,7 @@
         <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F16">
         <v>3800</v>
@@ -1112,10 +1217,13 @@
         <v>392</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
       <c r="C17" t="s">
         <v>54</v>
       </c>
@@ -1128,8 +1236,11 @@
       <c r="I17">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1137,7 +1248,7 @@
         <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
         <v>72</v>
@@ -1152,7 +1263,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1177,8 +1288,11 @@
       <c r="J19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1186,7 +1300,7 @@
         <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F20">
         <v>186</v>
@@ -1195,7 +1309,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1211,8 +1325,11 @@
       <c r="H21">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1234,8 +1351,11 @@
       <c r="G22">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1243,7 +1363,7 @@
         <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F23">
         <v>4.8</v>
@@ -1255,7 +1375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1269,7 +1389,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -1289,7 +1409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -1306,7 +1426,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1326,7 +1446,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -1346,7 +1466,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -1360,7 +1480,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -1368,7 +1488,7 @@
         <v>87</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E30" t="s">
         <v>86</v>
@@ -1376,8 +1496,11 @@
       <c r="H30">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -1397,7 +1520,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>93</v>
       </c>
@@ -1405,13 +1528,16 @@
         <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K32">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -1419,7 +1545,7 @@
         <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F33">
         <v>0.09</v>
@@ -1427,8 +1553,11 @@
       <c r="K33">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -1442,7 +1571,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -1450,7 +1579,7 @@
         <v>101</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E35" t="s">
         <v>100</v>
@@ -1460,6 +1589,30 @@
       </c>
       <c r="K35">
         <v>386</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>126</v>
+      </c>
+      <c r="L37" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="L38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>128</v>
+      </c>
+      <c r="L39" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Putting live the 'released' version of the site
</commit_message>
<xml_diff>
--- a/youtubers.xlsx
+++ b/youtubers.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="143">
   <si>
     <t>Name</t>
   </si>
@@ -450,6 +450,18 @@
   </si>
   <si>
     <t>XAL6Y-DGJQD-Z8A2P</t>
+  </si>
+  <si>
+    <t>KGPortal</t>
+  </si>
+  <si>
+    <t>WQKGN-FKV33-LRAI6</t>
+  </si>
+  <si>
+    <t>ECQWC-XXZRR-9TPWN</t>
+  </si>
+  <si>
+    <t>W8BG6-Y9J5V-KZJVJ</t>
   </si>
 </sst>
 </file>
@@ -821,11 +833,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M40" sqref="M40"/>
+      <selection pane="bottomLeft" activeCell="M41" sqref="M41:M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,6 +1783,24 @@
         <v>138</v>
       </c>
     </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>139</v>
+      </c>
+      <c r="M41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M1">
     <sortState ref="A2:M35">

</xml_diff>

<commit_message>
Updated todo and Excel file
</commit_message>
<xml_diff>
--- a/youtubers.xlsx
+++ b/youtubers.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -428,12 +428,6 @@
     <t>n</t>
   </si>
   <si>
-    <t>Made positive video</t>
-  </si>
-  <si>
-    <t>Made negative video</t>
-  </si>
-  <si>
     <t>Reminder email</t>
   </si>
   <si>
@@ -462,13 +456,34 @@
   </si>
   <si>
     <t>W8BG6-Y9J5V-KZJVJ</t>
+  </si>
+  <si>
+    <t>TOT game</t>
+  </si>
+  <si>
+    <t>KMDIG-99F0K-T0BLE</t>
+  </si>
+  <si>
+    <t>Tom Johnson</t>
+  </si>
+  <si>
+    <t> YMVKC-VGL02-RCXAL</t>
+  </si>
+  <si>
+    <t>Created video</t>
+  </si>
+  <si>
+    <t>Created negative video</t>
+  </si>
+  <si>
+    <t>0N2D5-62D32-WP7R5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +507,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -514,10 +535,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -833,11 +855,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M41" sqref="M41:M43"/>
+      <selection pane="bottomLeft" activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +927,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
         <v>130</v>
@@ -931,7 +953,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="E3" t="s">
         <v>129</v>
@@ -966,7 +988,7 @@
         <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
         <v>130</v>
@@ -989,7 +1011,7 @@
         <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E5" t="s">
         <v>130</v>
@@ -1015,7 +1037,7 @@
         <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E6" t="s">
         <v>130</v>
@@ -1041,13 +1063,13 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
         <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E7" t="s">
         <v>130</v>
@@ -1076,7 +1098,7 @@
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
         <v>130</v>
@@ -1099,7 +1121,7 @@
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="E9" t="s">
         <v>130</v>
@@ -1125,7 +1147,7 @@
         <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
         <v>130</v>
@@ -1214,7 +1236,7 @@
         <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E14" t="s">
         <v>130</v>
@@ -1240,7 +1262,7 @@
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E15" t="s">
         <v>130</v>
@@ -1269,7 +1291,7 @@
         <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s">
         <v>130</v>
@@ -1321,7 +1343,7 @@
         <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
         <v>130</v>
@@ -1333,7 +1355,7 @@
         <v>4</v>
       </c>
       <c r="M18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1347,7 +1369,7 @@
         <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="E19" t="s">
         <v>130</v>
@@ -1367,7 +1389,7 @@
         <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="E20" t="s">
         <v>130</v>
@@ -1399,7 +1421,7 @@
         <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E21" t="s">
         <v>130</v>
@@ -1428,7 +1450,7 @@
         <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E22" t="s">
         <v>130</v>
@@ -1483,7 +1505,7 @@
         <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E24" t="s">
         <v>130</v>
@@ -1561,7 +1583,7 @@
         <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E27" t="s">
         <v>130</v>
@@ -1584,7 +1606,7 @@
         <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E28" t="s">
         <v>130</v>
@@ -1607,7 +1629,7 @@
         <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E29" t="s">
         <v>130</v>
@@ -1627,7 +1649,7 @@
         <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E30" t="s">
         <v>130</v>
@@ -1650,7 +1672,7 @@
         <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E31" t="s">
         <v>130</v>
@@ -1670,7 +1692,7 @@
         <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E32" t="s">
         <v>130</v>
@@ -1690,7 +1712,7 @@
         <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E33" t="s">
         <v>130</v>
@@ -1710,13 +1732,16 @@
         <v>96</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E34" t="s">
         <v>130</v>
       </c>
       <c r="L34">
         <v>46</v>
+      </c>
+      <c r="M34" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -1777,28 +1802,44 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M40" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M41" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>141</v>
+      </c>
+      <c r="M44" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>143</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unsure what changed here
</commit_message>
<xml_diff>
--- a/youtubers.xlsx
+++ b/youtubers.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="150">
   <si>
     <t>Name</t>
   </si>
@@ -477,6 +477,12 @@
   </si>
   <si>
     <t>0N2D5-62D32-WP7R5</t>
+  </si>
+  <si>
+    <t>Maarten</t>
+  </si>
+  <si>
+    <t>8L8G8-LWVB5-LMPMF</t>
   </si>
 </sst>
 </file>
@@ -855,11 +861,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M34" sqref="M34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,6 +1848,14 @@
         <v>144</v>
       </c>
     </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>148</v>
+      </c>
+      <c r="M46" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M1">
     <sortState ref="A2:M35">

</xml_diff>